<commit_message>
adding audio to certain progams
</commit_message>
<xml_diff>
--- a/Source Workbooks/Sight word drills.xlsx
+++ b/Source Workbooks/Sight word drills.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ken\Desktop\ESLatHoward.com\Source Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F418BD71-1765-4F84-BFE0-82FC659FB3BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36E5C80-92FF-41B3-9EDA-ED7582FD4F3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sight25x3" sheetId="1" r:id="rId1"/>
+    <sheet name="Sight25x3 with Audio" sheetId="1" r:id="rId1"/>
     <sheet name="Sight100x3Feedback" sheetId="6" r:id="rId2"/>
     <sheet name="Sight100x3Test" sheetId="7" r:id="rId3"/>
     <sheet name="strip" sheetId="8" r:id="rId4"/>
@@ -26,19 +26,11 @@
     <externalReference r:id="rId9"/>
   </externalReferences>
   <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="160">
   <si>
     <t>(CHOICES)</t>
   </si>
@@ -122,12 +114,6 @@
   </si>
   <si>
     <t>25 SIGHT WORDS</t>
-  </si>
-  <si>
-    <t>click to hear</t>
-  </si>
-  <si>
-    <t>link</t>
   </si>
   <si>
     <t>Touch the word you hear</t>
@@ -901,7 +887,7 @@
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="169">
+  <cellXfs count="172">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1337,6 +1323,15 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -17951,16 +17946,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>182880</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>213360</xdr:rowOff>
+      <xdr:rowOff>281940</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>464820</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>259080</xdr:rowOff>
+      <xdr:rowOff>327660</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17989,7 +17984,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1501140" y="441960"/>
+          <a:off x="845820" y="510540"/>
           <a:ext cx="533400" cy="670560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -18608,8 +18603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:R32"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30:L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -18622,7 +18617,7 @@
     <col min="6" max="8" width="10.77734375" style="2" customWidth="1"/>
     <col min="9" max="10" width="1.77734375" style="2" customWidth="1"/>
     <col min="11" max="11" width="8.44140625" customWidth="1"/>
-    <col min="12" max="12" width="3.88671875" customWidth="1"/>
+    <col min="12" max="12" width="3.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:18" ht="23.4" x14ac:dyDescent="0.45">
@@ -18651,14 +18646,9 @@
         <f>[1]!wwsImage(Janice.jpg,0,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="B3" s="153" t="s">
-        <v>28</v>
-      </c>
+      <c r="B3" s="153"/>
       <c r="C3" s="153"/>
       <c r="D3" s="153"/>
-      <c r="O3" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="4" spans="1:18" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="150"/>
@@ -18711,6 +18701,7 @@
         <f t="shared" ref="K5:K29" si="1">IF(OR(A5=F5,A5=G5,A5=H5,A5=I5,A5=J5),"GOOD","")</f>
         <v>GOOD</v>
       </c>
+      <c r="L5" s="4"/>
       <c r="M5" s="12"/>
       <c r="O5" s="15"/>
       <c r="P5" s="15" t="s">
@@ -18755,6 +18746,7 @@
         <f t="shared" si="1"/>
         <v>GOOD</v>
       </c>
+      <c r="L6" s="4"/>
       <c r="R6" s="12"/>
     </row>
     <row r="7" spans="1:18" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -18794,6 +18786,7 @@
         <f t="shared" si="1"/>
         <v>GOOD</v>
       </c>
+      <c r="L7" s="4"/>
     </row>
     <row r="8" spans="1:18" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
@@ -18832,6 +18825,7 @@
         <f t="shared" si="1"/>
         <v>GOOD</v>
       </c>
+      <c r="L8" s="4"/>
     </row>
     <row r="9" spans="1:18" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
@@ -18870,7 +18864,7 @@
         <f t="shared" si="1"/>
         <v>GOOD</v>
       </c>
-      <c r="L9" s="13">
+      <c r="L9" s="170">
         <f>SUM(B5:B9)</f>
         <v>5</v>
       </c>
@@ -18912,6 +18906,7 @@
         <f t="shared" si="1"/>
         <v>GOOD</v>
       </c>
+      <c r="L10" s="4"/>
     </row>
     <row r="11" spans="1:18" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
@@ -18950,6 +18945,7 @@
         <f t="shared" si="1"/>
         <v>GOOD</v>
       </c>
+      <c r="L11" s="4"/>
     </row>
     <row r="12" spans="1:18" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
@@ -18988,6 +18984,7 @@
         <f t="shared" si="1"/>
         <v>GOOD</v>
       </c>
+      <c r="L12" s="4"/>
     </row>
     <row r="13" spans="1:18" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
@@ -19026,6 +19023,7 @@
         <f t="shared" si="1"/>
         <v>GOOD</v>
       </c>
+      <c r="L13" s="4"/>
     </row>
     <row r="14" spans="1:18" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
@@ -19064,7 +19062,7 @@
         <f t="shared" si="1"/>
         <v>GOOD</v>
       </c>
-      <c r="L14" s="13">
+      <c r="L14" s="170">
         <f>SUM(B10:B14)</f>
         <v>5</v>
       </c>
@@ -19106,6 +19104,7 @@
         <f t="shared" si="1"/>
         <v>GOOD</v>
       </c>
+      <c r="L15" s="4"/>
     </row>
     <row r="16" spans="1:18" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
@@ -19144,8 +19143,9 @@
         <f t="shared" si="1"/>
         <v>GOOD</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L16" s="4"/>
+    </row>
+    <row r="17" spans="1:16" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>15</v>
       </c>
@@ -19182,8 +19182,9 @@
         <f t="shared" si="1"/>
         <v>GOOD</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L17" s="4"/>
+    </row>
+    <row r="18" spans="1:16" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>14</v>
       </c>
@@ -19220,8 +19221,9 @@
         <f t="shared" si="1"/>
         <v>GOOD</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L18" s="4"/>
+    </row>
+    <row r="19" spans="1:16" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>9</v>
       </c>
@@ -19258,12 +19260,18 @@
         <f t="shared" si="1"/>
         <v>GOOD</v>
       </c>
-      <c r="L19" s="13">
+      <c r="L19" s="170">
         <f>SUM(B15:B19)</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M19" s="169" t="str">
+        <f>"&lt;audio style='width:100%; height:30px;' controls preload='metadata'&gt;&lt;source src='Sight_words_1-25_US_Female.mp3'/&gt;&lt;/audio&gt;"</f>
+        <v>&lt;audio style='width:100%; height:30px;' controls preload='metadata'&gt;&lt;source src='Sight_words_1-25_US_Female.mp3'/&gt;&lt;/audio&gt;</v>
+      </c>
+      <c r="N19" s="169"/>
+      <c r="O19" s="169"/>
+    </row>
+    <row r="20" spans="1:16" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>16</v>
       </c>
@@ -19300,8 +19308,9 @@
         <f t="shared" si="1"/>
         <v>GOOD</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L20" s="4"/>
+    </row>
+    <row r="21" spans="1:16" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>17</v>
       </c>
@@ -19338,8 +19347,9 @@
         <f t="shared" si="1"/>
         <v>GOOD</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L21" s="4"/>
+    </row>
+    <row r="22" spans="1:16" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>19</v>
       </c>
@@ -19376,8 +19386,9 @@
         <f t="shared" si="1"/>
         <v>GOOD</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L22" s="4"/>
+    </row>
+    <row r="23" spans="1:16" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>20</v>
       </c>
@@ -19414,8 +19425,9 @@
         <f t="shared" si="1"/>
         <v>GOOD</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L23" s="4"/>
+    </row>
+    <row r="24" spans="1:16" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>18</v>
       </c>
@@ -19452,12 +19464,12 @@
         <f t="shared" si="1"/>
         <v>GOOD</v>
       </c>
-      <c r="L24" s="13">
+      <c r="L24" s="170">
         <f>SUM(B20:B24)</f>
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:13" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>21</v>
       </c>
@@ -19494,8 +19506,9 @@
         <f t="shared" si="1"/>
         <v>GOOD</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L25" s="4"/>
+    </row>
+    <row r="26" spans="1:16" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>22</v>
       </c>
@@ -19532,8 +19545,9 @@
         <f t="shared" si="1"/>
         <v>GOOD</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L26" s="4"/>
+    </row>
+    <row r="27" spans="1:16" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>23</v>
       </c>
@@ -19570,8 +19584,9 @@
         <f t="shared" si="1"/>
         <v>GOOD</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L27" s="4"/>
+    </row>
+    <row r="28" spans="1:16" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>25</v>
       </c>
@@ -19608,8 +19623,9 @@
         <f t="shared" si="1"/>
         <v>GOOD</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L28" s="4"/>
+    </row>
+    <row r="29" spans="1:16" s="3" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>24</v>
       </c>
@@ -19646,30 +19662,30 @@
         <f t="shared" si="1"/>
         <v>GOOD</v>
       </c>
-      <c r="L29" s="13">
+      <c r="L29" s="170">
         <f>SUM(B25:B29)</f>
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" s="17"/>
       <c r="B30" s="18"/>
       <c r="C30" s="19"/>
-      <c r="K30" s="151">
+      <c r="K30" s="171">
         <f>SUM(B5:B29)/25</f>
         <v>1</v>
       </c>
-      <c r="L30" s="151"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="L30" s="171"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" s="17"/>
       <c r="B31" s="18"/>
       <c r="C31" s="19"/>
-      <c r="M31" t="s">
+      <c r="P31" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32" s="17"/>
       <c r="B32" s="18"/>
       <c r="C32" s="19"/>
@@ -19678,7 +19694,8 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G5:G29">
     <sortCondition ref="G5:G29"/>
   </sortState>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="M19:O19"/>
     <mergeCell ref="G4:I4"/>
     <mergeCell ref="K30:L30"/>
     <mergeCell ref="A2:F2"/>
@@ -20630,7 +20647,7 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="B3:D4" r:id="rId1" display="click to hear" xr:uid="{21E14C4B-E178-4238-AEDA-95B44A61C459}"/>
+    <hyperlink ref="M19" r:id="rId1" display="Sight words 1-25 US Female.mp3" xr:uid="{812BFA82-065D-4A45-A8DC-7FF64CA86E1E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -20682,7 +20699,7 @@
     </row>
     <row r="2" spans="1:21" ht="23.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="152" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B2" s="152"/>
       <c r="C2" s="152"/>
@@ -20704,7 +20721,7 @@
       <c r="M2" s="70"/>
       <c r="N2" s="70"/>
       <c r="O2" s="119" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="P2" s="119"/>
       <c r="Q2" s="70"/>
@@ -20729,10 +20746,10 @@
       <c r="M3" s="70"/>
       <c r="N3" s="70"/>
       <c r="O3" s="136" t="s">
+        <v>153</v>
+      </c>
+      <c r="P3" s="136" t="s">
         <v>155</v>
-      </c>
-      <c r="P3" s="136" t="s">
-        <v>157</v>
       </c>
       <c r="Q3" s="70"/>
       <c r="R3" s="70"/>
@@ -20767,7 +20784,7 @@
     </row>
     <row r="5" spans="1:21" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B5" s="133">
         <f>IF(I5="GOOD",1,0)</f>
@@ -20806,7 +20823,7 @@
       <c r="M5" s="8"/>
       <c r="N5" s="107"/>
       <c r="O5" s="120" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="P5" s="120" t="s">
         <v>16</v>
@@ -20861,7 +20878,7 @@
         <v>3</v>
       </c>
       <c r="P6" s="120" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="Q6" s="8"/>
       <c r="R6" s="8"/>
@@ -20871,7 +20888,7 @@
     </row>
     <row r="7" spans="1:21" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B7" s="133">
         <f t="shared" si="1"/>
@@ -20910,10 +20927,10 @@
       <c r="M7" s="109"/>
       <c r="N7" s="107"/>
       <c r="O7" s="120" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="P7" s="120" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="Q7" s="8"/>
       <c r="R7" s="8"/>
@@ -20923,7 +20940,7 @@
     </row>
     <row r="8" spans="1:21" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B8" s="133">
         <f t="shared" si="1"/>
@@ -20962,7 +20979,7 @@
       <c r="M8" s="109"/>
       <c r="N8" s="107"/>
       <c r="O8" s="120" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="P8" s="120" t="s">
         <v>7</v>
@@ -20975,7 +20992,7 @@
     </row>
     <row r="9" spans="1:21" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B9" s="133">
         <f t="shared" si="1"/>
@@ -21014,7 +21031,7 @@
       <c r="M9" s="109"/>
       <c r="N9" s="107"/>
       <c r="O9" s="120" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="P9" s="120" t="s">
         <v>3</v>
@@ -21027,7 +21044,7 @@
     </row>
     <row r="10" spans="1:21" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B10" s="133">
         <f t="shared" si="1"/>
@@ -21066,7 +21083,7 @@
       <c r="M10" s="109"/>
       <c r="N10" s="107"/>
       <c r="O10" s="120" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="P10" s="120" t="s">
         <v>2</v>
@@ -21079,7 +21096,7 @@
     </row>
     <row r="11" spans="1:21" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B11" s="133">
         <f t="shared" si="1"/>
@@ -21118,7 +21135,7 @@
       <c r="M11" s="109"/>
       <c r="N11" s="107"/>
       <c r="O11" s="120" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="P11" s="120" t="s">
         <v>10</v>
@@ -21183,7 +21200,7 @@
     </row>
     <row r="13" spans="1:21" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B13" s="133">
         <f t="shared" si="1"/>
@@ -21222,10 +21239,10 @@
       <c r="M13" s="109"/>
       <c r="N13" s="107"/>
       <c r="O13" s="120" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="P13" s="120" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="Q13" s="8"/>
       <c r="R13" s="8"/>
@@ -21235,7 +21252,7 @@
     </row>
     <row r="14" spans="1:21" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B14" s="133">
         <f t="shared" si="1"/>
@@ -21274,7 +21291,7 @@
       <c r="M14" s="109"/>
       <c r="N14" s="107"/>
       <c r="O14" s="120" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="P14" s="120" t="s">
         <v>9</v>
@@ -21287,7 +21304,7 @@
     </row>
     <row r="15" spans="1:21" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B15" s="133">
         <f t="shared" si="1"/>
@@ -21326,7 +21343,7 @@
       <c r="M15" s="109"/>
       <c r="N15" s="107"/>
       <c r="O15" s="120" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="P15" s="120" t="s">
         <v>12</v>
@@ -21339,7 +21356,7 @@
     </row>
     <row r="16" spans="1:21" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B16" s="133">
         <f t="shared" si="1"/>
@@ -21378,10 +21395,10 @@
       <c r="M16" s="109"/>
       <c r="N16" s="107"/>
       <c r="O16" s="120" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="P16" s="120" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="Q16" s="8"/>
       <c r="R16" s="8"/>
@@ -21391,7 +21408,7 @@
     </row>
     <row r="17" spans="1:21" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B17" s="133">
         <f t="shared" si="1"/>
@@ -21430,10 +21447,10 @@
       <c r="M17" s="109"/>
       <c r="N17" s="107"/>
       <c r="O17" s="120" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="P17" s="120" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="Q17" s="8"/>
       <c r="R17" s="8"/>
@@ -21443,7 +21460,7 @@
     </row>
     <row r="18" spans="1:21" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B18" s="133">
         <f t="shared" si="1"/>
@@ -21482,10 +21499,10 @@
       <c r="M18" s="109"/>
       <c r="N18" s="107"/>
       <c r="O18" s="120" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="P18" s="120" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="Q18" s="8"/>
       <c r="R18" s="8"/>
@@ -21495,7 +21512,7 @@
     </row>
     <row r="19" spans="1:21" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B19" s="133">
         <f t="shared" si="1"/>
@@ -21534,10 +21551,10 @@
       <c r="M19" s="109"/>
       <c r="N19" s="107"/>
       <c r="O19" s="120" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="P19" s="120" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="Q19" s="8"/>
       <c r="R19" s="8"/>
@@ -21641,7 +21658,7 @@
         <v>18</v>
       </c>
       <c r="P21" s="120" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="Q21" s="8"/>
       <c r="R21" s="8"/>
@@ -21651,7 +21668,7 @@
     </row>
     <row r="22" spans="1:21" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B22" s="133">
         <f t="shared" si="1"/>
@@ -21690,10 +21707,10 @@
       <c r="M22" s="109"/>
       <c r="N22" s="107"/>
       <c r="O22" s="120" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="P22" s="120" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="Q22" s="8"/>
       <c r="R22" s="8"/>
@@ -21703,7 +21720,7 @@
     </row>
     <row r="23" spans="1:21" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B23" s="133">
         <f t="shared" si="1"/>
@@ -21742,7 +21759,7 @@
       <c r="M23" s="109"/>
       <c r="N23" s="107"/>
       <c r="O23" s="120" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="P23" s="120" t="s">
         <v>16</v>
@@ -21755,7 +21772,7 @@
     </row>
     <row r="24" spans="1:21" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B24" s="133">
         <f t="shared" si="1"/>
@@ -21794,10 +21811,10 @@
       <c r="M24" s="109"/>
       <c r="N24" s="107"/>
       <c r="O24" s="120" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="P24" s="120" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="Q24" s="8"/>
       <c r="R24" s="8"/>
@@ -21807,7 +21824,7 @@
     </row>
     <row r="25" spans="1:21" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B25" s="133">
         <f t="shared" si="1"/>
@@ -21846,10 +21863,10 @@
       <c r="M25" s="109"/>
       <c r="N25" s="107"/>
       <c r="O25" s="120" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P25" s="120" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="Q25" s="8"/>
       <c r="R25" s="8"/>
@@ -21859,7 +21876,7 @@
     </row>
     <row r="26" spans="1:21" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B26" s="133">
         <f t="shared" si="1"/>
@@ -21898,10 +21915,10 @@
       <c r="M26" s="109"/>
       <c r="N26" s="107"/>
       <c r="O26" s="120" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="P26" s="120" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="Q26" s="8"/>
       <c r="R26" s="8"/>
@@ -21911,7 +21928,7 @@
     </row>
     <row r="27" spans="1:21" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B27" s="133">
         <f t="shared" si="1"/>
@@ -21950,10 +21967,10 @@
       <c r="M27" s="109"/>
       <c r="N27" s="107"/>
       <c r="O27" s="120" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="P27" s="120" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="Q27" s="8"/>
       <c r="R27" s="8"/>
@@ -21963,7 +21980,7 @@
     </row>
     <row r="28" spans="1:21" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B28" s="133">
         <f t="shared" si="1"/>
@@ -22002,10 +22019,10 @@
       <c r="M28" s="109"/>
       <c r="N28" s="107"/>
       <c r="O28" s="120" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="P28" s="120" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="Q28" s="8"/>
       <c r="R28" s="8"/>
@@ -22015,7 +22032,7 @@
     </row>
     <row r="29" spans="1:21" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B29" s="133">
         <f t="shared" si="1"/>
@@ -22054,10 +22071,10 @@
       <c r="M29" s="109"/>
       <c r="N29" s="107"/>
       <c r="O29" s="120" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="P29" s="120" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="Q29" s="8"/>
       <c r="R29" s="8"/>
@@ -22067,7 +22084,7 @@
     </row>
     <row r="30" spans="1:21" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B30" s="133">
         <f t="shared" si="1"/>
@@ -22106,7 +22123,7 @@
       <c r="M30" s="109"/>
       <c r="N30" s="107"/>
       <c r="O30" s="120" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="P30" s="120" t="s">
         <v>25</v>
@@ -22161,7 +22178,7 @@
         <v>4</v>
       </c>
       <c r="P31" s="120" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="Q31" s="8"/>
       <c r="R31" s="8"/>
@@ -25966,7 +25983,7 @@
     </row>
     <row r="2" spans="1:19" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A2" s="152" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B2" s="152"/>
       <c r="C2" s="152"/>
@@ -25988,7 +26005,7 @@
       <c r="M2" s="70"/>
       <c r="N2" s="70"/>
       <c r="O2" s="137" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="P2" s="137"/>
       <c r="Q2" s="70"/>
@@ -26010,10 +26027,10 @@
       <c r="M3" s="70"/>
       <c r="N3" s="70"/>
       <c r="O3" s="136" t="s">
+        <v>153</v>
+      </c>
+      <c r="P3" s="136" t="s">
         <v>155</v>
-      </c>
-      <c r="P3" s="136" t="s">
-        <v>157</v>
       </c>
       <c r="Q3" s="70"/>
       <c r="R3" s="70"/>
@@ -26042,7 +26059,7 @@
     </row>
     <row r="5" spans="1:19" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B5" s="139">
         <f>IF(I5="GOOD",1,0)</f>
@@ -26080,7 +26097,7 @@
       <c r="M5" s="123"/>
       <c r="N5" s="107"/>
       <c r="O5" s="120" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="P5" s="120" t="s">
         <v>16</v>
@@ -26133,7 +26150,7 @@
         <v>3</v>
       </c>
       <c r="P6" s="120" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="Q6" s="8"/>
       <c r="R6" s="8"/>
@@ -26141,7 +26158,7 @@
     </row>
     <row r="7" spans="1:19" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B7" s="139">
         <f t="shared" si="2"/>
@@ -26180,10 +26197,10 @@
       <c r="M7" s="123"/>
       <c r="N7" s="107"/>
       <c r="O7" s="120" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="P7" s="120" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="Q7" s="8"/>
       <c r="R7" s="8"/>
@@ -26191,7 +26208,7 @@
     </row>
     <row r="8" spans="1:19" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B8" s="139">
         <f t="shared" si="2"/>
@@ -26230,7 +26247,7 @@
       <c r="M8" s="123"/>
       <c r="N8" s="107"/>
       <c r="O8" s="120" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="P8" s="120" t="s">
         <v>7</v>
@@ -26241,7 +26258,7 @@
     </row>
     <row r="9" spans="1:19" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B9" s="139">
         <f t="shared" si="2"/>
@@ -26280,7 +26297,7 @@
       <c r="M9" s="123"/>
       <c r="N9" s="107"/>
       <c r="O9" s="120" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="P9" s="120" t="s">
         <v>3</v>
@@ -26291,7 +26308,7 @@
     </row>
     <row r="10" spans="1:19" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B10" s="139">
         <f t="shared" si="2"/>
@@ -26330,7 +26347,7 @@
       <c r="M10" s="123"/>
       <c r="N10" s="107"/>
       <c r="O10" s="120" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="P10" s="120" t="s">
         <v>2</v>
@@ -26341,7 +26358,7 @@
     </row>
     <row r="11" spans="1:19" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B11" s="139">
         <f t="shared" si="2"/>
@@ -26380,7 +26397,7 @@
       <c r="M11" s="123"/>
       <c r="N11" s="107"/>
       <c r="O11" s="120" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="P11" s="120" t="s">
         <v>10</v>
@@ -26441,7 +26458,7 @@
     </row>
     <row r="13" spans="1:19" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B13" s="139">
         <f t="shared" si="2"/>
@@ -26480,10 +26497,10 @@
       <c r="M13" s="123"/>
       <c r="N13" s="107"/>
       <c r="O13" s="120" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="P13" s="120" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="Q13" s="8"/>
       <c r="R13" s="8"/>
@@ -26491,7 +26508,7 @@
     </row>
     <row r="14" spans="1:19" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B14" s="139">
         <f t="shared" si="2"/>
@@ -26530,7 +26547,7 @@
       <c r="M14" s="123"/>
       <c r="N14" s="107"/>
       <c r="O14" s="120" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="P14" s="120" t="s">
         <v>9</v>
@@ -26541,7 +26558,7 @@
     </row>
     <row r="15" spans="1:19" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B15" s="139">
         <f t="shared" si="2"/>
@@ -26580,7 +26597,7 @@
       <c r="M15" s="123"/>
       <c r="N15" s="107"/>
       <c r="O15" s="120" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="P15" s="120" t="s">
         <v>12</v>
@@ -26591,7 +26608,7 @@
     </row>
     <row r="16" spans="1:19" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B16" s="139">
         <f t="shared" si="2"/>
@@ -26630,10 +26647,10 @@
       <c r="M16" s="123"/>
       <c r="N16" s="107"/>
       <c r="O16" s="120" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="P16" s="120" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="Q16" s="8"/>
       <c r="R16" s="8"/>
@@ -26641,7 +26658,7 @@
     </row>
     <row r="17" spans="1:19" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B17" s="139">
         <f t="shared" si="2"/>
@@ -26680,10 +26697,10 @@
       <c r="M17" s="123"/>
       <c r="N17" s="107"/>
       <c r="O17" s="120" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="P17" s="120" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="Q17" s="8"/>
       <c r="R17" s="8"/>
@@ -26691,7 +26708,7 @@
     </row>
     <row r="18" spans="1:19" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B18" s="139">
         <f t="shared" si="2"/>
@@ -26730,10 +26747,10 @@
       <c r="M18" s="123"/>
       <c r="N18" s="107"/>
       <c r="O18" s="120" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="P18" s="120" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="Q18" s="8"/>
       <c r="R18" s="8"/>
@@ -26741,7 +26758,7 @@
     </row>
     <row r="19" spans="1:19" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B19" s="139">
         <f t="shared" si="2"/>
@@ -26780,10 +26797,10 @@
       <c r="M19" s="123"/>
       <c r="N19" s="107"/>
       <c r="O19" s="120" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="P19" s="120" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="Q19" s="8"/>
       <c r="R19" s="8"/>
@@ -26883,7 +26900,7 @@
         <v>18</v>
       </c>
       <c r="P21" s="120" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="Q21" s="8"/>
       <c r="R21" s="8"/>
@@ -26891,7 +26908,7 @@
     </row>
     <row r="22" spans="1:19" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B22" s="139">
         <f t="shared" si="2"/>
@@ -26930,10 +26947,10 @@
       <c r="M22" s="123"/>
       <c r="N22" s="107"/>
       <c r="O22" s="120" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="P22" s="120" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="Q22" s="8"/>
       <c r="R22" s="8"/>
@@ -26941,7 +26958,7 @@
     </row>
     <row r="23" spans="1:19" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B23" s="139">
         <f t="shared" si="2"/>
@@ -26980,7 +26997,7 @@
       <c r="M23" s="123"/>
       <c r="N23" s="107"/>
       <c r="O23" s="120" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="P23" s="120" t="s">
         <v>16</v>
@@ -26991,7 +27008,7 @@
     </row>
     <row r="24" spans="1:19" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B24" s="139">
         <f t="shared" si="2"/>
@@ -27030,10 +27047,10 @@
       <c r="M24" s="123"/>
       <c r="N24" s="107"/>
       <c r="O24" s="120" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="P24" s="120" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="Q24" s="8"/>
       <c r="R24" s="8"/>
@@ -27041,7 +27058,7 @@
     </row>
     <row r="25" spans="1:19" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B25" s="139">
         <f t="shared" si="2"/>
@@ -27080,10 +27097,10 @@
       <c r="M25" s="123"/>
       <c r="N25" s="107"/>
       <c r="O25" s="120" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P25" s="120" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="Q25" s="8"/>
       <c r="R25" s="8"/>
@@ -27091,7 +27108,7 @@
     </row>
     <row r="26" spans="1:19" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B26" s="139">
         <f t="shared" si="2"/>
@@ -27130,10 +27147,10 @@
       <c r="M26" s="123"/>
       <c r="N26" s="107"/>
       <c r="O26" s="120" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="P26" s="120" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="Q26" s="8"/>
       <c r="R26" s="8"/>
@@ -27141,7 +27158,7 @@
     </row>
     <row r="27" spans="1:19" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B27" s="139">
         <f t="shared" si="2"/>
@@ -27180,10 +27197,10 @@
       <c r="M27" s="123"/>
       <c r="N27" s="107"/>
       <c r="O27" s="120" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="P27" s="120" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="Q27" s="8"/>
       <c r="R27" s="8"/>
@@ -27191,7 +27208,7 @@
     </row>
     <row r="28" spans="1:19" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B28" s="139">
         <f t="shared" si="2"/>
@@ -27230,10 +27247,10 @@
       <c r="M28" s="123"/>
       <c r="N28" s="107"/>
       <c r="O28" s="120" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="P28" s="120" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="Q28" s="8"/>
       <c r="R28" s="8"/>
@@ -27241,7 +27258,7 @@
     </row>
     <row r="29" spans="1:19" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B29" s="139">
         <f t="shared" si="2"/>
@@ -27280,10 +27297,10 @@
       <c r="M29" s="123"/>
       <c r="N29" s="107"/>
       <c r="O29" s="120" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="P29" s="120" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="Q29" s="8"/>
       <c r="R29" s="8"/>
@@ -27291,7 +27308,7 @@
     </row>
     <row r="30" spans="1:19" s="40" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B30" s="139">
         <f t="shared" si="2"/>
@@ -27330,7 +27347,7 @@
       <c r="M30" s="123"/>
       <c r="N30" s="107"/>
       <c r="O30" s="120" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="P30" s="120" t="s">
         <v>25</v>
@@ -27383,7 +27400,7 @@
         <v>4</v>
       </c>
       <c r="P31" s="120" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="Q31" s="8"/>
       <c r="R31" s="8"/>
@@ -28690,7 +28707,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="70" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B1" s="70"/>
       <c r="C1" s="70"/>
@@ -28708,7 +28725,7 @@
     </row>
     <row r="4" spans="1:10" ht="23.4" x14ac:dyDescent="0.45">
       <c r="F4" s="149" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G4" s="147" t="str">
         <f>G2</f>
@@ -28719,12 +28736,12 @@
         <v>hide</v>
       </c>
       <c r="I4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="23.4" x14ac:dyDescent="0.45">
       <c r="F5" s="149" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G5" s="147" t="s">
         <v>24</v>
@@ -28843,7 +28860,7 @@
       <c r="D4" s="157"/>
       <c r="E4" s="23"/>
       <c r="F4" s="155" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G4" s="155"/>
       <c r="H4" s="155"/>
@@ -31446,7 +31463,7 @@
       <c r="D4" s="153"/>
       <c r="E4" s="23"/>
       <c r="F4" s="160" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G4" s="160"/>
       <c r="H4" s="160"/>
@@ -31459,7 +31476,7 @@
     </row>
     <row r="5" spans="1:17" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B5" s="20">
         <f>IF(K5="GOOD",1,0)</f>
@@ -31506,7 +31523,7 @@
     </row>
     <row r="6" spans="1:17" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B6" s="20">
         <f t="shared" ref="B6:B29" si="2">IF(K6="GOOD",1,0)</f>
@@ -31553,7 +31570,7 @@
     </row>
     <row r="7" spans="1:17" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B7" s="20">
         <f t="shared" si="2"/>
@@ -31600,7 +31617,7 @@
     </row>
     <row r="8" spans="1:17" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B8" s="20">
         <f t="shared" si="2"/>
@@ -31647,7 +31664,7 @@
     </row>
     <row r="9" spans="1:17" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B9" s="20">
         <f t="shared" si="2"/>
@@ -31697,7 +31714,7 @@
     </row>
     <row r="10" spans="1:17" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B10" s="20">
         <f t="shared" si="2"/>
@@ -31744,7 +31761,7 @@
     </row>
     <row r="11" spans="1:17" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B11" s="20">
         <f t="shared" si="2"/>
@@ -31794,7 +31811,7 @@
     </row>
     <row r="12" spans="1:17" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B12" s="20">
         <f t="shared" si="2"/>
@@ -31844,7 +31861,7 @@
     </row>
     <row r="13" spans="1:17" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B13" s="20">
         <f t="shared" si="2"/>
@@ -31894,7 +31911,7 @@
     </row>
     <row r="14" spans="1:17" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B14" s="20">
         <f t="shared" si="2"/>
@@ -31947,7 +31964,7 @@
     </row>
     <row r="15" spans="1:17" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B15" s="20">
         <f t="shared" si="2"/>
@@ -31993,7 +32010,7 @@
     </row>
     <row r="16" spans="1:17" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B16" s="20">
         <f t="shared" si="2"/>
@@ -32039,7 +32056,7 @@
     </row>
     <row r="17" spans="1:13" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B17" s="20">
         <f t="shared" si="2"/>
@@ -32085,7 +32102,7 @@
     </row>
     <row r="18" spans="1:13" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B18" s="20">
         <f t="shared" si="2"/>
@@ -32131,7 +32148,7 @@
     </row>
     <row r="19" spans="1:13" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B19" s="20">
         <f t="shared" si="2"/>
@@ -32180,7 +32197,7 @@
     </row>
     <row r="20" spans="1:13" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B20" s="20">
         <f t="shared" si="2"/>
@@ -32226,7 +32243,7 @@
     </row>
     <row r="21" spans="1:13" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B21" s="20">
         <f t="shared" si="2"/>
@@ -32272,7 +32289,7 @@
     </row>
     <row r="22" spans="1:13" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B22" s="20">
         <f t="shared" si="2"/>
@@ -32318,7 +32335,7 @@
     </row>
     <row r="23" spans="1:13" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B23" s="20">
         <f t="shared" si="2"/>
@@ -32364,7 +32381,7 @@
     </row>
     <row r="24" spans="1:13" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B24" s="20">
         <f t="shared" si="2"/>
@@ -32413,7 +32430,7 @@
     </row>
     <row r="25" spans="1:13" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B25" s="20">
         <f t="shared" si="2"/>
@@ -32459,7 +32476,7 @@
     </row>
     <row r="26" spans="1:13" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B26" s="20">
         <f t="shared" si="2"/>
@@ -32505,7 +32522,7 @@
     </row>
     <row r="27" spans="1:13" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B27" s="20">
         <f t="shared" si="2"/>
@@ -32551,7 +32568,7 @@
     </row>
     <row r="28" spans="1:13" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B28" s="20">
         <f t="shared" si="2"/>
@@ -32597,7 +32614,7 @@
     </row>
     <row r="29" spans="1:13" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B29" s="20">
         <f t="shared" si="2"/>
@@ -34074,7 +34091,7 @@
     </row>
     <row r="2" spans="1:19" ht="27.6" x14ac:dyDescent="0.65">
       <c r="A2" s="161" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B2" s="161"/>
       <c r="C2" s="161"/>
@@ -34144,10 +34161,10 @@
     </row>
     <row r="5" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B5" s="74" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C5" s="37" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D5" s="36">
         <f>IF(J5=F5,1,0)</f>
@@ -34157,7 +34174,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="79" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G5" s="80" t="str">
         <f>[1]!wwsCheckbox(B5,3,FALSE)</f>
@@ -34198,10 +34215,10 @@
     </row>
     <row r="7" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B7" s="74" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D7" s="36">
         <f>IF(J7=F7,1,0)</f>
@@ -34211,7 +34228,7 @@
         <v>2</v>
       </c>
       <c r="F7" s="79" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G7" s="63" t="str">
         <f>[1]!wwsCheckbox(F7,31,FALSE)</f>
@@ -34251,10 +34268,10 @@
     </row>
     <row r="9" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B9" s="74" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D9" s="36">
         <f>IF(J9=F9,1,0)</f>
@@ -34264,7 +34281,7 @@
         <v>3</v>
       </c>
       <c r="F9" s="79" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G9" s="63" t="str">
         <f>[1]!wwsCheckbox(B9,32,FALSE)</f>
@@ -34304,10 +34321,10 @@
     </row>
     <row r="11" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B11" s="74" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C11" s="37" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D11" s="36">
         <f>IF(J11=F11,1,0)</f>
@@ -34317,7 +34334,7 @@
         <v>4</v>
       </c>
       <c r="F11" s="79" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G11" s="63" t="str">
         <f>[1]!wwsCheckbox(B11,33,FALSE)</f>
@@ -34357,10 +34374,10 @@
     </row>
     <row r="13" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B13" s="74" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D13" s="36">
         <f>IF(J13=F13,1,0)</f>
@@ -34370,7 +34387,7 @@
         <v>5</v>
       </c>
       <c r="F13" s="79" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G13" s="63" t="str">
         <f>[1]!wwsCheckbox(B13,34,FALSE)</f>
@@ -34410,10 +34427,10 @@
     </row>
     <row r="15" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B15" s="74" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C15" s="37" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D15" s="36">
         <f>IF(J15=F15,1,0)</f>
@@ -34423,7 +34440,7 @@
         <v>6</v>
       </c>
       <c r="F15" s="79" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G15" s="63" t="str">
         <f>[1]!wwsCheckbox(F15,35,FALSE)</f>
@@ -34463,10 +34480,10 @@
     </row>
     <row r="17" spans="2:16" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B17" s="74" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D17" s="36">
         <f>IF(J17=F17,1,0)</f>
@@ -34476,7 +34493,7 @@
         <v>7</v>
       </c>
       <c r="F17" s="79" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G17" s="63" t="str">
         <f>[1]!wwsCheckbox(B17,36,FALSE)</f>
@@ -40273,7 +40290,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5BEC25-7BD6-4F5F-A805-1C4467E721B9}">
   <dimension ref="A1:M163"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F4" sqref="F4:J4"/>
     </sheetView>
   </sheetViews>
@@ -40306,7 +40323,7 @@
     </row>
     <row r="2" spans="1:13" ht="27.6" x14ac:dyDescent="0.65">
       <c r="A2" s="161" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B2" s="161"/>
       <c r="C2" s="161"/>
@@ -40362,10 +40379,10 @@
     </row>
     <row r="5" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B5" s="74" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C5" s="37" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D5" s="36">
         <f>IF(J5=F5,1,0)</f>
@@ -40375,7 +40392,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="79" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G5" s="80" t="str">
         <f>[1]!wwsCheckbox(B5,5,FALSE)</f>
@@ -40413,10 +40430,10 @@
     </row>
     <row r="7" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B7" s="74" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D7" s="36">
         <f>IF(J7=F7,1,0)</f>
@@ -40426,7 +40443,7 @@
         <v>2</v>
       </c>
       <c r="F7" s="79" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G7" s="63" t="str">
         <f>[1]!wwsCheckbox(F7,7,FALSE)</f>
@@ -40464,10 +40481,10 @@
     </row>
     <row r="9" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B9" s="74" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D9" s="36">
         <f>IF(J9=F9,1,0)</f>
@@ -40477,7 +40494,7 @@
         <v>3</v>
       </c>
       <c r="F9" s="79" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G9" s="63" t="str">
         <f>[1]!wwsCheckbox(B9,9,FALSE)</f>
@@ -40515,10 +40532,10 @@
     </row>
     <row r="11" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B11" s="74" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C11" s="37" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D11" s="36">
         <f>IF(J11=F11,1,0)</f>
@@ -40528,7 +40545,7 @@
         <v>4</v>
       </c>
       <c r="F11" s="79" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G11" s="63" t="str">
         <f>[1]!wwsCheckbox(B11,11,FALSE)</f>
@@ -40566,10 +40583,10 @@
     </row>
     <row r="13" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B13" s="74" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="37" t="s">
         <v>78</v>
-      </c>
-      <c r="C13" s="37" t="s">
-        <v>80</v>
       </c>
       <c r="D13" s="36">
         <f>IF(J13=F13,1,0)</f>
@@ -40579,7 +40596,7 @@
         <v>5</v>
       </c>
       <c r="F13" s="79" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G13" s="63" t="str">
         <f>[1]!wwsCheckbox(B13,34,FALSE)</f>
@@ -40617,10 +40634,10 @@
     </row>
     <row r="15" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B15" s="74" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C15" s="37" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D15" s="36">
         <f>IF(J15=F15,1,0)</f>
@@ -40630,7 +40647,7 @@
         <v>6</v>
       </c>
       <c r="F15" s="79" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G15" s="63" t="str">
         <f>[1]!wwsCheckbox(F15,35,FALSE)</f>
@@ -40668,10 +40685,10 @@
     </row>
     <row r="17" spans="2:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B17" s="74" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D17" s="36">
         <f>IF(J17=F17,1,0)</f>
@@ -40681,7 +40698,7 @@
         <v>7</v>
       </c>
       <c r="F17" s="79" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G17" s="63" t="str">
         <f>[1]!wwsCheckbox(B17,17,FALSE)</f>
@@ -40719,10 +40736,10 @@
     </row>
     <row r="19" spans="2:13" ht="27.6" x14ac:dyDescent="0.35">
       <c r="B19" s="72" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C19" s="37" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D19" s="37">
         <f>IF(J19=F19,1,0)</f>
@@ -40732,7 +40749,7 @@
         <v>8</v>
       </c>
       <c r="F19" s="79" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G19" s="80" t="str">
         <f>[1]!wwsCheckbox(B19,19,FALSE)</f>
@@ -40770,10 +40787,10 @@
     </row>
     <row r="21" spans="2:13" ht="27.6" x14ac:dyDescent="0.35">
       <c r="B21" s="72" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C21" s="37" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D21" s="37">
         <f>IF(J21=F21,1,0)</f>
@@ -40821,10 +40838,10 @@
     </row>
     <row r="23" spans="2:13" ht="27.6" x14ac:dyDescent="0.35">
       <c r="B23" s="72" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C23" s="37" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D23" s="37">
         <f>IF(J23=F23,1,0)</f>
@@ -40835,7 +40852,7 @@
         <v>10</v>
       </c>
       <c r="F23" s="79" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G23" s="63" t="str">
         <f>[1]!wwsCheckbox(B23,23,FALSE)</f>
@@ -40873,10 +40890,10 @@
     </row>
     <row r="25" spans="2:13" ht="27.6" x14ac:dyDescent="0.35">
       <c r="B25" s="72" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C25" s="37" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D25" s="37">
         <f>IF(J25=F25,1,0)</f>
@@ -40887,7 +40904,7 @@
         <v>11</v>
       </c>
       <c r="F25" s="79" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G25" s="63" t="str">
         <f>[1]!wwsCheckbox(B25,25,FALSE)</f>
@@ -40928,7 +40945,7 @@
         <v>19</v>
       </c>
       <c r="C27" s="37" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D27" s="37">
         <f>IF(J27=F27,1,0)</f>
@@ -40939,7 +40956,7 @@
         <v>12</v>
       </c>
       <c r="F27" s="79" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G27" s="63" t="str">
         <f>[1]!wwsCheckbox(B27,27,FALSE)</f>
@@ -40977,10 +40994,10 @@
     </row>
     <row r="29" spans="2:13" ht="27.6" x14ac:dyDescent="0.35">
       <c r="B29" s="72" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C29" s="37" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D29" s="37">
         <f>IF(J29=F29,1,0)</f>
@@ -40991,7 +41008,7 @@
         <v>13</v>
       </c>
       <c r="F29" s="79" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G29" s="63" t="str">
         <f>[1]!wwsCheckbox(F29,29,FALSE)</f>
@@ -41029,10 +41046,10 @@
     </row>
     <row r="31" spans="2:13" ht="27.6" x14ac:dyDescent="0.35">
       <c r="B31" s="72" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C31" s="37" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D31" s="37">
         <f>IF(J31=F31,1,0)</f>
@@ -41043,7 +41060,7 @@
         <v>14</v>
       </c>
       <c r="F31" s="79" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G31" s="63" t="str">
         <f>[1]!wwsCheckbox(B31,31,FALSE)</f>
@@ -41081,10 +41098,10 @@
     </row>
     <row r="33" spans="2:13" ht="27.6" x14ac:dyDescent="0.35">
       <c r="B33" s="72" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" s="37" t="s">
         <v>73</v>
-      </c>
-      <c r="C33" s="37" t="s">
-        <v>75</v>
       </c>
       <c r="D33" s="37">
         <f>IF(J33=F33,1,0)</f>
@@ -41095,7 +41112,7 @@
         <v>15</v>
       </c>
       <c r="F33" s="79" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G33" s="80" t="str">
         <f>[1]!wwsCheckbox(B33,3,FALSE)</f>
@@ -41133,10 +41150,10 @@
     </row>
     <row r="35" spans="2:13" ht="27.6" x14ac:dyDescent="0.35">
       <c r="B35" s="72" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C35" s="37" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D35" s="37">
         <f>IF(J35=F35,1,0)</f>
@@ -41147,7 +41164,7 @@
         <v>16</v>
       </c>
       <c r="F35" s="79" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G35" s="63" t="str">
         <f>[1]!wwsCheckbox(F35,4,FALSE)</f>
@@ -41185,10 +41202,10 @@
     </row>
     <row r="37" spans="2:13" ht="27.6" x14ac:dyDescent="0.35">
       <c r="B37" s="72" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C37" s="37" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D37" s="37">
         <f>IF(J37=F37,1,0)</f>
@@ -41199,7 +41216,7 @@
         <v>17</v>
       </c>
       <c r="F37" s="79" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G37" s="63" t="str">
         <f>[1]!wwsCheckbox(B37,37,FALSE)</f>
@@ -41237,10 +41254,10 @@
     </row>
     <row r="39" spans="2:13" ht="27.6" x14ac:dyDescent="0.35">
       <c r="B39" s="72" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C39" s="37" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D39" s="37">
         <f>IF(J39=F39,1,0)</f>
@@ -41251,7 +41268,7 @@
         <v>18</v>
       </c>
       <c r="F39" s="79" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G39" s="63" t="str">
         <f>[1]!wwsCheckbox(B39,39,FALSE)</f>
@@ -41289,7 +41306,7 @@
     </row>
     <row r="41" spans="2:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B41" s="72" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C41" s="37">
         <v>2</v>
@@ -41303,7 +41320,7 @@
         <v>19</v>
       </c>
       <c r="F41" s="79" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G41" s="63" t="str">
         <f>[1]!wwsCheckbox(B41,41,FALSE)</f>
@@ -41344,7 +41361,7 @@
         <v>19</v>
       </c>
       <c r="C43" s="37" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D43" s="37">
         <f>IF(J43=F43,1,0)</f>
@@ -41355,7 +41372,7 @@
         <v>20</v>
       </c>
       <c r="F43" s="79" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G43" s="63" t="str">
         <f>[1]!wwsCheckbox(F43,43,,FALSE)</f>
@@ -41393,10 +41410,10 @@
     </row>
     <row r="45" spans="2:13" ht="36.6" x14ac:dyDescent="0.3">
       <c r="B45" s="72" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C45" s="37" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D45" s="37">
         <f>IF(J45=F45,1,0)</f>
@@ -41407,7 +41424,7 @@
         <v>21</v>
       </c>
       <c r="F45" s="79" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G45" s="88" t="str">
         <f>[1]!wwsCheckbox(B45,45,FALSE)</f>
@@ -41445,10 +41462,10 @@
     </row>
     <row r="47" spans="2:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B47" s="72" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C47" s="37" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D47" s="37">
         <f>IF(J47=F47,1,0)</f>
@@ -41459,7 +41476,7 @@
         <v>22</v>
       </c>
       <c r="F47" s="79" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G47" s="80" t="str">
         <f>[1]!wwsCheckbox(B47,47,FALSE)</f>
@@ -41497,10 +41514,10 @@
     </row>
     <row r="49" spans="2:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B49" s="72" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C49" s="37" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D49" s="37">
         <f>IF(J49=F49,1,0)</f>
@@ -41511,7 +41528,7 @@
         <v>23</v>
       </c>
       <c r="F49" s="79" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G49" s="63" t="str">
         <f>[1]!wwsCheckbox(F49,49,FALSE)</f>
@@ -41549,10 +41566,10 @@
     </row>
     <row r="51" spans="2:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B51" s="72" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C51" s="37" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D51" s="37">
         <f>IF(J51=F51,1,0)</f>
@@ -41563,7 +41580,7 @@
         <v>24</v>
       </c>
       <c r="F51" s="79" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G51" s="63" t="str">
         <f>[1]!wwsCheckbox(B51,51,FALSE)</f>
@@ -41601,10 +41618,10 @@
     </row>
     <row r="53" spans="2:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B53" s="72" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C53" s="37" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D53" s="37">
         <f>IF(J53=F53,1,0)</f>
@@ -41615,7 +41632,7 @@
         <v>25</v>
       </c>
       <c r="F53" s="79" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G53" s="63" t="str">
         <f>[1]!wwsCheckbox(B53,53,FALSE)</f>
@@ -41653,10 +41670,10 @@
     </row>
     <row r="55" spans="2:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B55" s="72" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C55" s="37" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D55" s="37">
         <f>IF(J55=F55,1,0)</f>
@@ -41667,7 +41684,7 @@
         <v>26</v>
       </c>
       <c r="F55" s="79" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G55" s="63" t="str">
         <f>[1]!wwsCheckbox(B55,55,FALSE)</f>
@@ -41708,10 +41725,10 @@
     </row>
     <row r="57" spans="2:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B57" s="74" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C57" s="37" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D57" s="37">
         <f>IF(J57=F57,1,0)</f>
@@ -41759,10 +41776,10 @@
     </row>
     <row r="59" spans="2:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B59" s="74" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C59" s="37" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D59" s="36">
         <f>IF(J59=F59,1,0)</f>
@@ -41773,7 +41790,7 @@
         <v>28</v>
       </c>
       <c r="F59" s="79" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G59" s="63" t="str">
         <f>[1]!wwsCheckbox(F59,59,FALSE)</f>
@@ -41811,10 +41828,10 @@
     </row>
     <row r="61" spans="2:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B61" s="74" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C61" s="37" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D61" s="36">
         <f>IF(J61=F61,1,0)</f>
@@ -41825,7 +41842,7 @@
         <v>29</v>
       </c>
       <c r="F61" s="79" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G61" s="63" t="str">
         <f>[1]!wwsCheckbox(B61,61,FALSE)</f>
@@ -41863,10 +41880,10 @@
     </row>
     <row r="63" spans="2:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B63" s="74" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C63" s="37" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D63" s="36">
         <f>IF(J63=F63,1,0)</f>
@@ -41877,7 +41894,7 @@
         <v>30</v>
       </c>
       <c r="F63" s="79" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G63" s="63" t="str">
         <f>[1]!wwsCheckbox(B63,63,FALSE)</f>
@@ -41915,10 +41932,10 @@
     </row>
     <row r="65" spans="2:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B65" s="74" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C65" s="37" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D65" s="36">
         <f>IF(J65=F65,1,0)</f>
@@ -41929,7 +41946,7 @@
         <v>31</v>
       </c>
       <c r="F65" s="79" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G65" s="63" t="str">
         <f>[1]!wwsCheckbox(B65,65,FALSE)</f>
@@ -41967,10 +41984,10 @@
     </row>
     <row r="67" spans="2:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B67" s="74" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C67" s="37" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D67" s="36">
         <f>IF(J67=F67,1,0)</f>
@@ -41980,7 +41997,7 @@
         <v>32</v>
       </c>
       <c r="F67" s="79" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G67" s="63" t="str">
         <f>[1]!wwsCheckbox(F67,67,FALSE)</f>
@@ -42018,7 +42035,7 @@
     </row>
     <row r="69" spans="2:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B69" s="74" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C69" s="37">
         <v>9</v>
@@ -42032,7 +42049,7 @@
         <v>33</v>
       </c>
       <c r="F69" s="79" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G69" s="63" t="str">
         <f>[1]!wwsCheckbox(B69,69,FALSE)</f>
@@ -42078,7 +42095,7 @@
         <v>34</v>
       </c>
       <c r="F71" s="79" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G71" s="80" t="str">
         <f>[1]!wwsCheckbox(B69,71,FALSE)</f>
@@ -42116,7 +42133,7 @@
     </row>
     <row r="73" spans="2:13" ht="27.6" x14ac:dyDescent="0.35">
       <c r="B73" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C73" s="1">
         <v>1</v>
@@ -42130,7 +42147,7 @@
         <v>35</v>
       </c>
       <c r="F73" s="79" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G73" s="80" t="str">
         <f>[1]!wwsCheckbox(B73,73,FALSE)</f>
@@ -42168,10 +42185,10 @@
     </row>
     <row r="75" spans="2:13" ht="27.6" x14ac:dyDescent="0.35">
       <c r="B75" s="72" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C75" s="37" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D75" s="36">
         <f>IF(J75=F75,1,0)</f>
@@ -42182,7 +42199,7 @@
         <v>36</v>
       </c>
       <c r="F75" s="79" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G75" s="63" t="str">
         <f>[1]!wwsCheckbox(F75,75,FALSE)</f>
@@ -42220,10 +42237,10 @@
     </row>
     <row r="77" spans="2:13" ht="27.6" x14ac:dyDescent="0.35">
       <c r="B77" s="72" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C77" s="37" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D77" s="36">
         <f>IF(J77=F77,1,0)</f>
@@ -42234,7 +42251,7 @@
         <v>37</v>
       </c>
       <c r="F77" s="79" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G77" s="63" t="str">
         <f>[1]!wwsCheckbox(B77,77,FALSE)</f>
@@ -42275,7 +42292,7 @@
         <v>1</v>
       </c>
       <c r="C79" s="37" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D79" s="36">
         <f>IF(J79=F79,1,0)</f>
@@ -42286,7 +42303,7 @@
         <v>38</v>
       </c>
       <c r="F79" s="79" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G79" s="63">
         <f>[1]!wwsCheckbox(B79,79,FALSE)</f>
@@ -42324,10 +42341,10 @@
     </row>
     <row r="81" spans="2:13" ht="27.6" x14ac:dyDescent="0.35">
       <c r="B81" s="72" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C81" s="37" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D81" s="36">
         <f>IF(J81=F81,1,0)</f>
@@ -42338,7 +42355,7 @@
         <v>39</v>
       </c>
       <c r="F81" s="79" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G81" s="63" t="str">
         <f>[1]!wwsCheckbox(B81,81,FALSE)</f>
@@ -42376,10 +42393,10 @@
     </row>
     <row r="83" spans="2:13" ht="27.6" x14ac:dyDescent="0.35">
       <c r="B83" s="72" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C83" s="37" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D83" s="36">
         <f>IF(J83=F83,1,0)</f>
@@ -42390,7 +42407,7 @@
         <v>40</v>
       </c>
       <c r="F83" s="79" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G83" s="63" t="str">
         <f>[1]!wwsCheckbox(F83,83,FALSE)</f>
@@ -42428,10 +42445,10 @@
     </row>
     <row r="85" spans="2:13" ht="27.6" x14ac:dyDescent="0.35">
       <c r="B85" s="72" t="s">
+        <v>95</v>
+      </c>
+      <c r="C85" s="37" t="s">
         <v>97</v>
-      </c>
-      <c r="C85" s="37" t="s">
-        <v>99</v>
       </c>
       <c r="D85" s="36">
         <f>IF(J85=F85,1,0)</f>
@@ -42442,7 +42459,7 @@
         <v>41</v>
       </c>
       <c r="F85" s="79" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G85" s="63" t="str">
         <f>[1]!wwsCheckbox(B85,85,FALSE)</f>
@@ -42480,10 +42497,10 @@
     </row>
     <row r="87" spans="2:13" ht="27.6" x14ac:dyDescent="0.35">
       <c r="B87" s="72" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C87" s="37" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D87" s="36">
         <f>IF(J87=F87,1,0)</f>
@@ -42494,7 +42511,7 @@
         <v>42</v>
       </c>
       <c r="F87" s="79" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G87" s="80" t="str">
         <f>[1]!wwsCheckbox(B87,87,FALSE)</f>
@@ -42532,10 +42549,10 @@
     </row>
     <row r="89" spans="2:13" ht="27.6" x14ac:dyDescent="0.35">
       <c r="B89" s="72" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C89" s="37" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D89" s="36">
         <f>IF(J89=F89,1,0)</f>
@@ -42546,7 +42563,7 @@
         <v>43</v>
       </c>
       <c r="F89" s="79" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G89" s="63" t="str">
         <f>[1]!wwsCheckbox(F89,89,FALSE)</f>
@@ -42584,10 +42601,10 @@
     </row>
     <row r="91" spans="2:13" ht="27.6" x14ac:dyDescent="0.35">
       <c r="B91" s="72" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C91" s="37" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D91" s="36">
         <f>IF(J91=F91,1,0)</f>
@@ -42598,7 +42615,7 @@
         <v>44</v>
       </c>
       <c r="F91" s="79" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G91" s="63" t="str">
         <f>[1]!wwsCheckbox(B91,91,FALSE)</f>
@@ -42636,10 +42653,10 @@
     </row>
     <row r="93" spans="2:13" ht="27.6" x14ac:dyDescent="0.35">
       <c r="B93" s="72" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C93" s="37" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D93" s="36">
         <f>IF(J93=F93,1,0)</f>
@@ -42650,7 +42667,7 @@
         <v>45</v>
       </c>
       <c r="F93" s="79" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G93" s="63" t="str">
         <f>[1]!wwsCheckbox(B93,93,FALSE)</f>
@@ -42688,10 +42705,10 @@
     </row>
     <row r="95" spans="2:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B95" s="72" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C95" s="37" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D95" s="36">
         <f>IF(J95=F95,1,0)</f>
@@ -42702,7 +42719,7 @@
         <v>46</v>
       </c>
       <c r="F95" s="79" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G95" s="63" t="str">
         <f>[1]!wwsCheckbox(B95,95,FALSE)</f>
@@ -42740,10 +42757,10 @@
     </row>
     <row r="97" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B97" s="72" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C97" s="37" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D97" s="36">
         <f>IF(J97=F97,1,0)</f>
@@ -42754,7 +42771,7 @@
         <v>47</v>
       </c>
       <c r="F97" s="79" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G97" s="63" t="str">
         <f>[1]!wwsCheckbox(F97,97,FALSE)</f>
@@ -42792,10 +42809,10 @@
     </row>
     <row r="99" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B99" s="72" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C99" s="37" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D99" s="36">
         <f>IF(J99=F99,1,0)</f>
@@ -42806,7 +42823,7 @@
         <v>48</v>
       </c>
       <c r="F99" s="79" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G99" s="63" t="str">
         <f>[1]!wwsCheckbox(B99,99,FALSE)</f>
@@ -42844,10 +42861,10 @@
     </row>
     <row r="101" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B101" s="72" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C101" s="37" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D101" s="36">
         <f>IF(J101=F101,1,0)</f>
@@ -42858,7 +42875,7 @@
         <v>49</v>
       </c>
       <c r="F101" s="79" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G101" s="80" t="str">
         <f>[1]!wwsCheckbox(B101,98,FALSE)</f>
@@ -42896,10 +42913,10 @@
     </row>
     <row r="103" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B103" s="72" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C103" s="37" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D103" s="36">
         <f>IF(J103=F103,1,0)</f>
@@ -42910,7 +42927,7 @@
         <v>50</v>
       </c>
       <c r="F103" s="79" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G103" s="63" t="str">
         <f>[1]!wwsCheckbox(F103,96,FALSE)</f>
@@ -42948,10 +42965,10 @@
     </row>
     <row r="105" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B105" s="72" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C105" s="37" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D105" s="36">
         <f>IF(J105=F105,1,0)</f>
@@ -42962,7 +42979,7 @@
         <v>51</v>
       </c>
       <c r="F105" s="79" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G105" s="63" t="str">
         <f>[1]!wwsCheckbox(B105,94,FALSE)</f>
@@ -43000,7 +43017,7 @@
     </row>
     <row r="107" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B107" s="72" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C107" s="37">
         <v>2</v>
@@ -43014,7 +43031,7 @@
         <v>52</v>
       </c>
       <c r="F107" s="79" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G107" s="63" t="str">
         <f>[1]!wwsCheckbox(B107,92,FALSE)</f>
@@ -43041,10 +43058,10 @@
     </row>
     <row r="108" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B108" s="74" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C108" s="37" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D108" s="36"/>
       <c r="E108" s="47"/>
@@ -43062,10 +43079,10 @@
         <v>1</v>
       </c>
       <c r="B109" s="72" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C109" s="37" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D109" s="36">
         <f>IF(OR(A109=G109,A109=H109,A109=I109),1,0)</f>
@@ -43076,7 +43093,7 @@
         <v>53</v>
       </c>
       <c r="F109" s="79" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G109" s="63" t="str">
         <f>[1]!wwsCheckbox(B109,90,FALSE)</f>
@@ -43114,13 +43131,13 @@
     </row>
     <row r="111" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B111" s="74" t="s">
         <v>96</v>
       </c>
-      <c r="B111" s="74" t="s">
-        <v>98</v>
-      </c>
       <c r="C111" s="37" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D111" s="36">
         <f>IF(OR(A111=G111,A111=H111,A111=I111),1,0)</f>
@@ -43131,7 +43148,7 @@
         <v>54</v>
       </c>
       <c r="F111" s="79" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G111" s="80" t="str">
         <f>[1]!wwsCheckbox(A111,88,FALSE)</f>
@@ -43169,13 +43186,13 @@
     </row>
     <row r="113" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B113" s="74" t="s">
+        <v>111</v>
+      </c>
+      <c r="C113" s="37" t="s">
         <v>97</v>
-      </c>
-      <c r="B113" s="74" t="s">
-        <v>113</v>
-      </c>
-      <c r="C113" s="37" t="s">
-        <v>99</v>
       </c>
       <c r="D113" s="36">
         <f>IF(OR(F113=UPPER(G113),F113=UPPER(H113),F113=UPPER(I113)),1,0)</f>
@@ -43186,7 +43203,7 @@
         <v>55</v>
       </c>
       <c r="F113" s="79" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G113" s="63" t="str">
         <f>[1]!wwsCheckbox(B113,86,FALSE)</f>
@@ -43224,13 +43241,13 @@
     </row>
     <row r="115" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B115" s="74" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C115" s="37" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D115" s="36">
         <f>IF(OR(F115=UPPER(G115),F115=UPPER(H115),F115=UPPER(I115)),1,0)</f>
@@ -43241,7 +43258,7 @@
         <v>56</v>
       </c>
       <c r="F115" s="79" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G115" s="63" t="str">
         <f>[1]!wwsCheckbox(B115,84,FALSE)</f>
@@ -43279,13 +43296,13 @@
     </row>
     <row r="117" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B117" s="74" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C117" s="37" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D117" s="36">
         <f>IF(OR(F117=UPPER(G117),F117=UPPER(H117),F117=UPPER(I117)),1,0)</f>
@@ -43296,7 +43313,7 @@
         <v>57</v>
       </c>
       <c r="F117" s="79" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G117" s="63" t="str">
         <f>[1]!wwsCheckbox(B117,82,FALSE)</f>
@@ -43334,13 +43351,13 @@
     </row>
     <row r="119" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B119" s="74" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C119" s="37" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D119" s="36">
         <f>IF(OR(F119=UPPER(G119),F119=UPPER(H119),F119=UPPER(I119)),1,0)</f>
@@ -43351,7 +43368,7 @@
         <v>58</v>
       </c>
       <c r="F119" s="79" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G119" s="80" t="str">
         <f>[1]!wwsCheckbox(A119,80,FALSE)</f>
@@ -43389,13 +43406,13 @@
     </row>
     <row r="121" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B121" s="74">
         <v>6</v>
       </c>
       <c r="C121" s="37" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D121" s="36">
         <f>IF(OR(F121=UPPER(G121),F121=UPPER(H121),F121=UPPER(I121)),1,0)</f>
@@ -43406,7 +43423,7 @@
         <v>59</v>
       </c>
       <c r="F121" s="79" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G121" s="63">
         <f>[1]!wwsCheckbox(B121,78,FALSE)</f>
@@ -43444,13 +43461,13 @@
     </row>
     <row r="123" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B123" s="72" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C123" s="37" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D123" s="36">
         <f>IF(OR(F123=UPPER(G123),F123=UPPER(H123),F123=UPPER(I123)),1,0)</f>
@@ -43461,7 +43478,7 @@
         <v>60</v>
       </c>
       <c r="F123" s="79" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G123" s="80" t="str">
         <f>[1]!wwsCheckbox(B123,76,FALSE)</f>
@@ -43499,13 +43516,13 @@
     </row>
     <row r="125" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B125" s="72">
         <v>1</v>
       </c>
       <c r="C125" s="37" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D125" s="36">
         <f>IF(OR(F125=UPPER(G125),F125=UPPER(H125),F125=UPPER(I125)),1,0)</f>
@@ -43554,13 +43571,13 @@
     </row>
     <row r="127" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B127" s="72" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C127" s="37" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D127" s="36">
         <f>IF(OR(F127=UPPER(G127),F127=UPPER(H127),F127=UPPER(I127)),1,0)</f>
@@ -43571,7 +43588,7 @@
         <v>62</v>
       </c>
       <c r="F127" s="79" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G127" s="63" t="str">
         <f>[1]!wwsCheckbox(B127,72,FALSE)</f>
@@ -43609,13 +43626,13 @@
     </row>
     <row r="129" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B129" s="72" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C129" s="37" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D129" s="36">
         <f>IF(OR(F129=UPPER(G129),F129=UPPER(H129),F129=UPPER(I129)),1,0)</f>
@@ -43626,7 +43643,7 @@
         <v>63</v>
       </c>
       <c r="F129" s="79" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G129" s="63" t="str">
         <f>[1]!wwsCheckbox(B129,70,FALSE)</f>
@@ -43664,13 +43681,13 @@
     </row>
     <row r="131" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B131" s="72" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C131" s="37" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D131" s="36">
         <f>IF(OR(F131=UPPER(G131),F131=UPPER(H131),F131=UPPER(I131)),1,0)</f>
@@ -43681,7 +43698,7 @@
         <v>64</v>
       </c>
       <c r="F131" s="79" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G131" s="63" t="str">
         <f>[1]!wwsCheckbox(B131,68,FALSE)</f>
@@ -43719,13 +43736,13 @@
     </row>
     <row r="133" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B133" s="72" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C133" s="37" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D133" s="36">
         <f>IF(OR(F133=UPPER(G133),F133=UPPER(H133),F133=UPPER(I133)),1,0)</f>
@@ -43736,7 +43753,7 @@
         <v>65</v>
       </c>
       <c r="F133" s="79" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G133" s="80" t="str">
         <f>[1]!wwsCheckbox(A133,66,FALSE)</f>
@@ -43774,13 +43791,13 @@
     </row>
     <row r="135" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B135" s="72" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C135" s="37" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D135" s="36">
         <f>IF(OR(F135=UPPER(G135),F135=UPPER(H135),F135=UPPER(I135)),1,0)</f>
@@ -43791,7 +43808,7 @@
         <v>66</v>
       </c>
       <c r="F135" s="79" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G135" s="63" t="str">
         <f>[1]!wwsCheckbox(B135,64,FALSE)</f>
@@ -43829,13 +43846,13 @@
     </row>
     <row r="137" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B137" s="72" t="s">
         <v>1</v>
       </c>
       <c r="C137" s="37" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D137" s="36">
         <f>IF(OR(F137=UPPER(G137),F137=UPPER(H137),F137=UPPER(I137)),1,0)</f>
@@ -43846,7 +43863,7 @@
         <v>67</v>
       </c>
       <c r="F137" s="79" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G137" s="80" t="str">
         <f>[1]!wwsCheckbox(B137,16,FALSE)</f>
@@ -43881,13 +43898,13 @@
     </row>
     <row r="139" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B139" s="72" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C139" s="37" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D139" s="36">
         <f>IF(OR(F139=UPPER(G139),F139=UPPER(H139),F139=UPPER(I139)),1,0)</f>
@@ -43898,7 +43915,7 @@
         <v>68</v>
       </c>
       <c r="F139" s="79" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G139" s="80" t="str">
         <f>[1]!wwsCheckbox(A139,62,FALSE)</f>
@@ -43933,13 +43950,13 @@
     </row>
     <row r="141" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B141" s="72" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C141" s="37" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D141" s="36">
         <f>IF(OR(F141=UPPER(G141),F141=UPPER(H141),F141=UPPER(I141)),1,0)</f>
@@ -43950,7 +43967,7 @@
         <v>69</v>
       </c>
       <c r="F141" s="79" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G141" s="63" t="str">
         <f>[1]!wwsCheckbox(B141,60,FALSE)</f>
@@ -43985,13 +44002,13 @@
     </row>
     <row r="143" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B143" s="72" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C143" s="37" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D143" s="36">
         <f>IF(OR(F143=UPPER(G143),F143=UPPER(H143),F143=UPPER(I143)),1,0)</f>
@@ -44002,7 +44019,7 @@
         <v>70</v>
       </c>
       <c r="F143" s="79" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G143" s="63" t="str">
         <f>[1]!wwsCheckbox(B143,58,FALSE)</f>
@@ -44037,13 +44054,13 @@
     </row>
     <row r="145" spans="1:13" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B145" s="72">
         <v>2</v>
       </c>
       <c r="C145" s="37" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D145" s="36">
         <f>IF(OR(F145=UPPER(G145),F145=UPPER(H145),F145=UPPER(I145)),1,0)</f>
@@ -44054,7 +44071,7 @@
         <v>71</v>
       </c>
       <c r="F145" s="79" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G145" s="63">
         <f>[1]!wwsCheckbox(B145,56,FALSE)</f>
@@ -44089,13 +44106,13 @@
     </row>
     <row r="147" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B147" s="72" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C147" s="37" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D147" s="36">
         <f>IF(OR(F147=UPPER(G147),F147=UPPER(H147),F147=UPPER(I147)),1,0)</f>
@@ -44106,7 +44123,7 @@
         <v>72</v>
       </c>
       <c r="F147" s="79" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G147" s="80" t="str">
         <f>[1]!wwsCheckbox(A147,100,FALSE)</f>
@@ -44141,13 +44158,13 @@
     </row>
     <row r="149" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B149" s="72" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C149" s="37" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D149" s="36">
         <f>IF(OR(F149=UPPER(G149),F149=UPPER(H149),F149=UPPER(I149)),1,0)</f>
@@ -44158,7 +44175,7 @@
         <v>73</v>
       </c>
       <c r="F149" s="79" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G149" s="63" t="str">
         <f>[1]!wwsCheckbox(B149,50,FALSE)</f>
@@ -44193,13 +44210,13 @@
     </row>
     <row r="151" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B151" s="72" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C151" s="37" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D151" s="36">
         <f>IF(OR(F151=UPPER(G151),F151=UPPER(H151),F151=UPPER(I151)),1,0)</f>
@@ -44210,7 +44227,7 @@
         <v>74</v>
       </c>
       <c r="F151" s="79" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G151" s="80" t="str">
         <f>[1]!wwsCheckbox(B151,48,FALSE)</f>
@@ -44245,13 +44262,13 @@
     </row>
     <row r="153" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B153" s="72" t="s">
         <v>117</v>
       </c>
-      <c r="B153" s="72" t="s">
-        <v>119</v>
-      </c>
       <c r="C153" s="37" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D153" s="36">
         <f>IF(OR(F153=UPPER(G153),F153=UPPER(H153),F153=UPPER(I153)),1,0)</f>
@@ -44262,7 +44279,7 @@
         <v>75</v>
       </c>
       <c r="F153" s="79" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G153" s="80" t="str">
         <f>[1]!wwsCheckbox(A153,46,FALSE)</f>
@@ -44297,13 +44314,13 @@
     </row>
     <row r="155" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B155" s="72" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C155" s="37" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D155" s="36">
         <f>IF(OR(F155=UPPER(G155),F155=UPPER(H155),F155=UPPER(I155)),1,0)</f>
@@ -44314,7 +44331,7 @@
         <v>76</v>
       </c>
       <c r="F155" s="79" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G155" s="63" t="str">
         <f>[1]!wwsCheckbox(B155,44,FALSE)</f>
@@ -44349,13 +44366,13 @@
     </row>
     <row r="157" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B157" s="72" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C157" s="37" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D157" s="36">
         <f>IF(OR(F157=UPPER(G157),F157=UPPER(H157),F157=UPPER(I157)),1,0)</f>
@@ -44366,7 +44383,7 @@
         <v>77</v>
       </c>
       <c r="F157" s="79" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G157" s="63" t="str">
         <f>[1]!wwsCheckbox(B157,42,FALSE)</f>
@@ -44401,13 +44418,13 @@
     </row>
     <row r="159" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B159" s="1">
         <v>2</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D159" s="36">
         <f>IF(OR(F159=UPPER(G159),F159=UPPER(H159),F159=UPPER(I159)),1,0)</f>
@@ -44418,7 +44435,7 @@
         <v>78</v>
       </c>
       <c r="F159" s="79" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G159" s="63">
         <f>[1]!wwsCheckbox(B159,40,FALSE)</f>

</xml_diff>

<commit_message>
still having F12 https errors
</commit_message>
<xml_diff>
--- a/Source Workbooks/Sight word drills.xlsx
+++ b/Source Workbooks/Sight word drills.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ken\Desktop\ESLatHoward.com\Source Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E38EEE73-1F76-47E8-8628-D6C84533EB5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D40EA5-97F9-4424-A26B-39D0B5698973}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sight25x3 with Audio" sheetId="1" r:id="rId1"/>
@@ -18665,7 +18665,7 @@
   <dimension ref="A2:R32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>

</xml_diff>